<commit_message>
New sample kind BUFFY COAT and new container tube box 21x10
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_v3_5_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_v3_5_0.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t xml:space="preserve">Container Creation Template</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tube box 10x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tube box 21x10</t>
   </si>
   <si>
     <t xml:space="preserve">Tube rack 8x12</t>
@@ -464,7 +467,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
@@ -4795,7 +4798,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A8:A107" type="list">
-      <formula1>Index!$A$2:$A$24</formula1>
+      <formula1>Index!$A$2:$A$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4820,7 +4823,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>
@@ -4861,18 +4864,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4881,7 +4884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -4906,7 +4909,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>23</v>
       </c>
@@ -4921,7 +4924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>26</v>
       </c>
@@ -4931,19 +4934,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>